<commit_message>
remove error for statistics
</commit_message>
<xml_diff>
--- a/160216_한반도 영향평가를 위한 변수 목록_최종안.xlsx
+++ b/160216_한반도 영향평가를 위한 변수 목록_최종안.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\code\east_asia\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15090" windowHeight="10485"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15090" windowHeight="10490"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -862,34 +862,34 @@
   <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="3.25" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="6.08203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="4.75" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="5.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.58203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="5.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.83203125" style="7" customWidth="1"/>
     <col min="12" max="13" width="4.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="53.625" style="9" customWidth="1"/>
-    <col min="15" max="15" width="56.375" style="9" customWidth="1"/>
-    <col min="16" max="16" width="58.375" style="9" customWidth="1"/>
-    <col min="17" max="17" width="11.125" style="4" customWidth="1"/>
-    <col min="18" max="18" width="5.375" style="4" customWidth="1"/>
-    <col min="19" max="19" width="6.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="53.58203125" style="9" customWidth="1"/>
+    <col min="15" max="15" width="56.33203125" style="9" customWidth="1"/>
+    <col min="16" max="16" width="58.33203125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="11.08203125" style="4" customWidth="1"/>
+    <col min="18" max="18" width="5.33203125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="42.5" style="5" customWidth="1"/>
     <col min="21" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="36.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="20" t="s">
         <v>17</v>
       </c>
@@ -924,7 +924,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="48" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
@@ -984,7 +984,7 @@
       </c>
       <c r="T2" s="21"/>
     </row>
-    <row r="3" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1249,7 +1249,7 @@
       </c>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="7">
         <v>12</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="7">
         <v>14</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -1631,7 +1631,7 @@
       </c>
       <c r="S17" s="3"/>
     </row>
-    <row r="18" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
         <v>16</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="11">
         <v>17</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="11">
         <v>18</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="14" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" s="14" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="11">
         <v>19</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="14" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" s="14" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="11">
         <v>20</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="14" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" s="14" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
         <v>21</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="11">
         <v>22</v>
       </c>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="S24" s="3"/>
     </row>
-    <row r="25" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
         <v>23</v>
       </c>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="S25" s="3"/>
     </row>
-    <row r="26" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="11">
         <v>24</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
         <v>25</v>
       </c>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="S27" s="7"/>
     </row>
-    <row r="28" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="11">
         <v>26</v>
       </c>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="R28" s="7"/>
     </row>
-    <row r="29" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
         <v>27</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="11">
         <v>28</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
         <v>29</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="11">
         <v>30</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="11">
         <v>31</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="11">
         <v>32</v>
       </c>
@@ -2399,32 +2399,32 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.45">
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A36" s="5"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.45">
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.45">
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.45">
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.45">
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.45">
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.45">
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.45">
       <c r="C43" s="1"/>
     </row>
   </sheetData>

</xml_diff>